<commit_message>
Part 1 of report 1 done
</commit_message>
<xml_diff>
--- a/Assignment 2/Computabillity/report/spreadsheet.xlsx
+++ b/Assignment 2/Computabillity/report/spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Bsc Computing\Science Of Computing\Assignment 2\Computabillity\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5B0D08-7114-43FE-A210-E2E69B0B7C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DDCC97-4217-4DFF-804E-15D348912DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15960" yWindow="8340" windowWidth="36885" windowHeight="19455" xr2:uid="{E4D5BD64-F78E-47C3-BF5E-854A0244FFDC}"/>
+    <workbookView xWindow="17175" yWindow="855" windowWidth="36885" windowHeight="19455" xr2:uid="{E4D5BD64-F78E-47C3-BF5E-854A0244FFDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -817,7 +817,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Size (Number of Intetgers)</a:t>
+                  <a:t> Size (Number of Integers)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -1809,7 +1809,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Dataset Size (Number of Intetgers)</a:t>
+                  <a:t>Dataset Size (Number of Integers)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2821,7 +2821,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Dataset Size (Number of Intetgers)</a:t>
+                  <a:t>Dataset Size (Number of Integers)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3833,7 +3833,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Dataset Size (Number of Intetgers)</a:t>
+                  <a:t>Dataset Size (Number of Integers)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6834,8 +6834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F396B2CD-6DA0-4DBC-914F-8346A4C190DC}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP28" sqref="AP28"/>
+    <sheetView tabSelected="1" topLeftCell="J28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X48" sqref="X48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>